<commit_message>
test cases changed at 12.58
</commit_message>
<xml_diff>
--- a/bin/in/v2solutions/hybrid/tsmodules/VWR_TestCases.xlsx
+++ b/bin/in/v2solutions/hybrid/tsmodules/VWR_TestCases.xlsx
@@ -1963,7 +1963,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2006,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2017,7 +2017,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2028,7 +2028,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2039,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
changes done at 2.20
</commit_message>
<xml_diff>
--- a/bin/in/v2solutions/hybrid/tsmodules/VWR_TestCases.xlsx
+++ b/bin/in/v2solutions/hybrid/tsmodules/VWR_TestCases.xlsx
@@ -1963,7 +1963,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2105,7 +2105,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>